<commit_message>
Treat composite keys as multiple simple keys
</commit_message>
<xml_diff>
--- a/tests/xlsx/default.xlsx
+++ b/tests/xlsx/default.xlsx
@@ -203,7 +203,7 @@
     <t>main_id</t>
   </si>
   <si>
-    <t>main_integer_minmax</t>
+    <t>main_string_enum</t>
   </si>
   <si>
     <t>a</t>
@@ -705,7 +705,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -719,9 +719,22 @@
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF(ISBLANK(A2), FALSE, IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE))</formula>
-    </cfRule>
-  </conditionalFormatting>
+      <formula>IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), ISNA(MATCH(A2, 'main'!$A$2:$A$1048576, 0))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>IF(ISBLANK(B2), FALSE, ISNA(MATCH(B2, 'main'!$F$2:$F$1048576, 0)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="A2:A1048576">
+      <formula1>'main'!$A$2:$A$1048576</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="B2:B1048576">
+      <formula1>'main'!$F$2:$F$1048576</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add support for Google Sheets
Also includes adjustments brought on by this addition:
* Adjustments to data validation error message wording and formatting
* Move of Layout.indirect to Layout method arguments
* Minor bug fixes and refactoring
* Additions to docstrings
</commit_message>
<xml_diff>
--- a/tests/xlsx/default.xlsx
+++ b/tests/xlsx/default.xlsx
@@ -646,10 +646,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="D2:D1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="D2:D1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="F2:F1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="F2:F1048576">
       <formula1>'lists'!$A$1:$A$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -684,7 +684,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="A2:A1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="A2:A1048576">
       <formula1>'main'!$A$2:$A$1048576</formula1>
     </dataValidation>
   </dataValidations>
@@ -728,10 +728,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="A2:A1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="A2:A1048576">
       <formula1>'main'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in dropdown list" sqref="B2:B1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="B2:B1048576">
       <formula1>'main'!$F$2:$F$1048576</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Test integer and number enum constraints
</commit_message>
<xml_diff>
--- a/tests/xlsx/default.xlsx
+++ b/tests/xlsx/default.xlsx
@@ -113,6 +113,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>One of the first three positive integers</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>One of the first three quarters after 1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -177,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -198,6 +224,12 @@
   </si>
   <si>
     <t>string_pattern</t>
+  </si>
+  <si>
+    <t>integer_enum</t>
+  </si>
+  <si>
+    <t>number_enum</t>
   </si>
   <si>
     <t>main_id</t>
@@ -573,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -589,9 +621,11 @@
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,12 +646,18 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$G2) &lt;&gt; 7), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$I2) &lt;&gt; 9), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
@@ -645,12 +685,28 @@
       <formula>IF(ISBLANK(F2), FALSE, ISNA(MATCH(F2, 'lists'!$A$1:$A$3, 0)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>IF(ISBLANK(H2), FALSE, OR(IF(ISNUMBER(H2), INT(H2) &lt;&gt; H2, TRUE), ISNA(MATCH(H2, 'lists'!$B$1:$B$3, 0))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>IF(ISBLANK(I2), FALSE, OR(NOT(ISNUMBER(I2)), ISNA(MATCH(I2, 'lists'!$C$1:$C$3, 0))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="D2:D1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="F2:F1048576">
       <formula1>'lists'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="H2:H1048576">
+      <formula1>'lists'!$B$1:$B$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="I2:I1048576">
+      <formula1>'lists'!$C$1:$C$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -674,7 +730,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -710,10 +766,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -742,25 +798,43 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1.25</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set column widths based on font size and style
Uses glyph widths from the Arial and Calibri fonts to set column widths
based on the font size and style of the header row.
This is exact for Google Sheets, but is approximate for Excel since it
assumes the default font is the same as the requested font family
in regular style and size 11.
</commit_message>
<xml_diff>
--- a/tests/xlsx/default.xlsx
+++ b/tests/xlsx/default.xlsx
@@ -302,7 +302,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,15 +616,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -725,7 +727,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -760,8 +762,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
Format header row and set column widths (#7)
* Set header row height
* Set column widths
* Vertical align header to top by default
* Set column widths based on font, size, and style

Uses glyph widths from select fonts to set column widths based on header row formatting.
This is exact for Google Sheets, but is approximate for Excel because it assumes the user default is Calibri 11 pt regular,
and because conversion from pixels to character units is fraught.
</commit_message>
<xml_diff>
--- a/tests/xlsx/default.xlsx
+++ b/tests/xlsx/default.xlsx
@@ -302,7 +302,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,15 +616,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -725,7 +727,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -760,8 +762,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>